<commit_message>
Results from July 2, 2020 7:40 pm CT run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-02.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-02.xlsx
@@ -70,74 +70,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -430,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,29 +430,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44013</v>
       </c>
       <c r="C2" t="n">
-        <v>109143</v>
+        <v>144013</v>
       </c>
       <c r="D2" t="n">
-        <v>8081</v>
+        <v>6951</v>
       </c>
       <c r="E2" t="n">
-        <v>10242</v>
+        <v>24191</v>
       </c>
       <c r="F2" t="n">
-        <v>664</v>
+        <v>1934</v>
       </c>
       <c r="G2" t="n">
-        <v>9.380000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="H2" t="n">
-        <v>8.220000000000001</v>
+        <v>27.82</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -541,16 +473,16 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C3" t="n">
-        <v>33435</v>
+        <v>34151</v>
       </c>
       <c r="D3" t="n">
-        <v>1339</v>
+        <v>1342</v>
       </c>
       <c r="E3" t="n">
-        <v>1366</v>
+        <v>1381</v>
       </c>
       <c r="F3" t="n">
         <v>43</v>
@@ -576,35 +508,35 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C4" t="n">
-        <v>33029</v>
+        <v>68142</v>
       </c>
       <c r="D4" t="n">
-        <v>1697</v>
+        <v>1391</v>
       </c>
       <c r="E4" t="n">
-        <v>1776</v>
+        <v>11075</v>
       </c>
       <c r="F4" t="n">
-        <v>109</v>
+        <v>445</v>
       </c>
       <c r="G4" t="n">
-        <v>5.38</v>
+        <v>16.25</v>
       </c>
       <c r="H4" t="n">
-        <v>6.48</v>
+        <v>31.99</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -615,35 +547,39 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
         <v>44014</v>
       </c>
-      <c r="C5" t="n">
-        <v>166303</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3617</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>212774</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>18519</t>
+        </is>
       </c>
       <c r="E5" t="n">
-        <v>23157</v>
+        <v>33093</v>
       </c>
       <c r="F5" t="n">
-        <v>709</v>
+        <v>5171</v>
       </c>
       <c r="G5" t="n">
-        <v>13.92</v>
+        <v>30.17</v>
       </c>
       <c r="H5" t="n">
-        <v>19.6</v>
+        <v>30.48</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -654,26 +590,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C6" t="n">
-        <v>3328</v>
+        <v>29738</v>
       </c>
       <c r="D6" t="n">
-        <v>105</v>
+        <v>793</v>
       </c>
       <c r="E6" t="n">
-        <v>790</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>5174</v>
+      </c>
+      <c r="F6" t="n">
+        <v>188</v>
+      </c>
       <c r="G6" t="n">
-        <v>26.87</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
+        <v>19.4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>24.04</v>
+      </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
@@ -689,35 +629,35 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C7" t="n">
-        <v>84237</v>
+        <v>11672</v>
       </c>
       <c r="D7" t="n">
-        <v>2827</v>
+        <v>355</v>
       </c>
       <c r="E7" t="n">
-        <v>23908</v>
+        <v>3405</v>
       </c>
       <c r="F7" t="n">
-        <v>1338</v>
+        <v>143</v>
       </c>
       <c r="G7" t="n">
-        <v>28.38</v>
+        <v>33.42</v>
       </c>
       <c r="H7" t="n">
-        <v>47.33</v>
+        <v>40.28</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -728,35 +668,35 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mississippi</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44014</v>
+        <v>44011</v>
       </c>
       <c r="C8" t="n">
-        <v>28770</v>
+        <v>16226</v>
       </c>
       <c r="D8" t="n">
-        <v>530</v>
+        <v>946</v>
       </c>
       <c r="E8" t="n">
-        <v>14137</v>
+        <v>1573</v>
       </c>
       <c r="F8" t="n">
-        <v>1109</v>
+        <v>47</v>
       </c>
       <c r="G8" t="n">
-        <v>49.14</v>
+        <v>12.33</v>
       </c>
       <c r="H8" t="n">
-        <v>209.25</v>
+        <v>6.11</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -767,35 +707,35 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44012</v>
+        <v>44014</v>
       </c>
       <c r="C9" t="n">
-        <v>105507</v>
+        <v>46890</v>
       </c>
       <c r="D9" t="n">
-        <v>3402</v>
+        <v>620</v>
       </c>
       <c r="E9" t="n">
-        <v>2904</v>
+        <v>9850</v>
       </c>
       <c r="F9" t="n">
-        <v>358</v>
+        <v>217</v>
       </c>
       <c r="G9" t="n">
-        <v>2.75</v>
+        <v>21.01</v>
       </c>
       <c r="H9" t="n">
-        <v>10.52</v>
+        <v>35</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -806,41 +746,31 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44013</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>22716</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>173</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>613</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>&lt;5</t>
-        </is>
-      </c>
+        <v>44014</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3328</v>
+      </c>
+      <c r="D10" t="n">
+        <v>105</v>
+      </c>
+      <c r="E10" t="n">
+        <v>790</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>2.7</v>
+        <v>26.87</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -851,29 +781,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C11" t="n">
-        <v>11553</v>
+        <v>68423</v>
       </c>
       <c r="D11" t="n">
-        <v>355</v>
+        <v>3086</v>
       </c>
       <c r="E11" t="n">
-        <v>3289</v>
+        <v>19474</v>
       </c>
       <c r="F11" t="n">
-        <v>143</v>
+        <v>1246</v>
       </c>
       <c r="G11" t="n">
-        <v>30.77</v>
+        <v>28.46</v>
       </c>
       <c r="H11" t="n">
-        <v>40.28</v>
+        <v>40.38</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -890,32 +820,32 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C12" t="n">
-        <v>21960</v>
+        <v>39604</v>
       </c>
       <c r="D12" t="n">
-        <v>662</v>
+        <v>961</v>
       </c>
       <c r="E12" t="n">
-        <v>2592</v>
+        <v>14595</v>
       </c>
       <c r="F12" t="n">
-        <v>85</v>
+        <v>436</v>
       </c>
       <c r="G12" t="n">
-        <v>1180.33</v>
+        <v>47.04</v>
       </c>
       <c r="H12" t="n">
-        <v>1283.99</v>
+        <v>46.88</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -929,35 +859,35 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44009</v>
+        <v>44014</v>
       </c>
       <c r="C13" t="n">
-        <v>20261</v>
+        <v>64596</v>
       </c>
       <c r="D13" t="n">
-        <v>996</v>
+        <v>5888</v>
       </c>
       <c r="E13" t="n">
-        <v>5758</v>
+        <v>19767</v>
       </c>
       <c r="F13" t="n">
-        <v>246</v>
+        <v>2356</v>
       </c>
       <c r="G13" t="n">
-        <v>49.66</v>
+        <v>30.6</v>
       </c>
       <c r="H13" t="n">
-        <v>38.56</v>
+        <v>40.01</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -968,30 +898,26 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C14" t="n">
-        <v>63735</v>
+        <v>1083</v>
       </c>
       <c r="D14" t="n">
-        <v>1816</v>
+        <v>22</v>
       </c>
       <c r="E14" t="n">
-        <v>9195</v>
-      </c>
-      <c r="F14" t="n">
-        <v>396</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>14.43</v>
-      </c>
-      <c r="H14" t="n">
-        <v>21.81</v>
-      </c>
+        <v>0.55</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
         <v>1</v>
       </c>
@@ -1007,35 +933,35 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44011</v>
+        <v>44014</v>
       </c>
       <c r="C15" t="n">
-        <v>16226</v>
+        <v>1017</v>
       </c>
       <c r="D15" t="n">
-        <v>946</v>
+        <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>1573</v>
+        <v>24</v>
       </c>
       <c r="F15" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>12.33</v>
+        <v>2.36</v>
       </c>
       <c r="H15" t="n">
-        <v>6.11</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1046,35 +972,35 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C16" t="n">
-        <v>10390</v>
+        <v>109338</v>
       </c>
       <c r="D16" t="n">
-        <v>554</v>
+        <v>8132</v>
       </c>
       <c r="E16" t="n">
-        <v>5174</v>
+        <v>10283</v>
       </c>
       <c r="F16" t="n">
-        <v>408</v>
+        <v>665</v>
       </c>
       <c r="G16" t="n">
-        <v>49.8</v>
+        <v>9.4</v>
       </c>
       <c r="H16" t="n">
-        <v>73.65000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1085,35 +1011,35 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Delaware</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44014</v>
+        <v>44009</v>
       </c>
       <c r="C17" t="n">
-        <v>11731</v>
+        <v>20261</v>
       </c>
       <c r="D17" t="n">
-        <v>510</v>
+        <v>996</v>
       </c>
       <c r="E17" t="n">
-        <v>3060</v>
+        <v>5758</v>
       </c>
       <c r="F17" t="n">
-        <v>131</v>
+        <v>246</v>
       </c>
       <c r="G17" t="n">
-        <v>26.08</v>
+        <v>49.66</v>
       </c>
       <c r="H17" t="n">
-        <v>25.69</v>
+        <v>38.56</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1124,32 +1050,38 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
         <v>44014</v>
       </c>
-      <c r="C18" t="n">
-        <v>39604</v>
-      </c>
-      <c r="D18" t="n">
-        <v>961</v>
-      </c>
-      <c r="E18" t="n">
-        <v>14595</v>
-      </c>
-      <c r="F18" t="n">
-        <v>436</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>23270</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
       </c>
       <c r="G18" t="n">
-        <v>47.04</v>
-      </c>
-      <c r="H18" t="n">
-        <v>46.88</v>
-      </c>
+        <v>2.7</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1163,31 +1095,35 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C19" t="n">
-        <v>12276</v>
+        <v>28770</v>
       </c>
       <c r="D19" t="n">
-        <v>500</v>
+        <v>530</v>
       </c>
       <c r="E19" t="n">
-        <v>232</v>
-      </c>
-      <c r="F19" t="inlineStr"/>
+        <v>14137</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1109</v>
+      </c>
       <c r="G19" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="H19" t="inlineStr"/>
+        <v>49.14</v>
+      </c>
+      <c r="H19" t="n">
+        <v>209.25</v>
+      </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
       <c r="J19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -1198,35 +1134,35 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C20" t="n">
-        <v>1227</v>
+        <v>12878</v>
       </c>
       <c r="D20" t="n">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="E20" t="n">
-        <v>118</v>
+        <v>464</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G20" t="n">
-        <v>9.880000000000001</v>
+        <v>6.81</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>15.32</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1237,35 +1173,35 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C21" t="n">
-        <v>64057</v>
+        <v>37210</v>
       </c>
       <c r="D21" t="n">
-        <v>5873</v>
+        <v>1458</v>
       </c>
       <c r="E21" t="n">
-        <v>19687</v>
+        <v>7707</v>
       </c>
       <c r="F21" t="n">
-        <v>2352</v>
+        <v>125</v>
       </c>
       <c r="G21" t="n">
-        <v>30.73</v>
+        <v>20.71</v>
       </c>
       <c r="H21" t="n">
-        <v>40.05</v>
+        <v>8.57</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1276,35 +1212,35 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C22" t="n">
-        <v>978</v>
+        <v>22341</v>
       </c>
       <c r="D22" t="n">
-        <v>14</v>
+        <v>662</v>
       </c>
       <c r="E22" t="n">
-        <v>24</v>
+        <v>2630</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G22" t="n">
-        <v>2.45</v>
+        <v>0.12</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -1315,47 +1251,35 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44013</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>159300</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>5983</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>6953</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>561</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4.4</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>9.4</t>
-        </is>
+        <v>44014</v>
+      </c>
+      <c r="C23" t="n">
+        <v>11731</v>
+      </c>
+      <c r="D23" t="n">
+        <v>510</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3060</v>
+      </c>
+      <c r="F23" t="n">
+        <v>131</v>
+      </c>
+      <c r="G23" t="n">
+        <v>26.08</v>
+      </c>
+      <c r="H23" t="n">
+        <v>25.69</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -1366,60 +1290,86 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Maryland</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+          <t>Nebraska</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C24" t="n">
+        <v>19452</v>
+      </c>
+      <c r="D24" t="n">
+        <v>282</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1127</v>
+      </c>
+      <c r="F24" t="n">
+        <v>21</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7.89</v>
+      </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>An error occurred. ... OSError(8, 'Exec format error')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
         <v>44013</v>
       </c>
-      <c r="C25" t="n">
-        <v>14623</v>
-      </c>
-      <c r="D25" t="n">
-        <v>372</v>
-      </c>
-      <c r="E25" t="n">
-        <v>506</v>
-      </c>
-      <c r="F25" t="n">
-        <v>12</v>
-      </c>
-      <c r="G25" t="n">
-        <v>4.35</v>
-      </c>
-      <c r="H25" t="n">
-        <v>3.26</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>159300</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>5983</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6953</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>561</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>9.4</t>
+        </is>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -1430,32 +1380,32 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C26" t="n">
-        <v>37210</v>
+        <v>1227</v>
       </c>
       <c r="D26" t="n">
-        <v>1458</v>
+        <v>56</v>
       </c>
       <c r="E26" t="n">
-        <v>7707</v>
+        <v>118</v>
       </c>
       <c r="F26" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>20.71</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="H26" t="n">
-        <v>8.57</v>
+        <v>0</v>
       </c>
       <c r="I26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="b">
         <v>1</v>
@@ -1469,35 +1419,31 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C27" t="n">
-        <v>15842</v>
+        <v>12520</v>
       </c>
       <c r="D27" t="n">
-        <v>572</v>
+        <v>503</v>
       </c>
       <c r="E27" t="n">
-        <v>1566</v>
-      </c>
-      <c r="F27" t="n">
-        <v>86</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>14.37</v>
-      </c>
-      <c r="H27" t="n">
-        <v>16.07</v>
-      </c>
+        <v>1.96</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -1508,54 +1454,68 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>North Carolina</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C28" t="n">
+        <v>166303</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3617</v>
+      </c>
+      <c r="E28" t="n">
+        <v>23157</v>
+      </c>
+      <c r="F28" t="n">
+        <v>709</v>
+      </c>
+      <c r="G28" t="n">
+        <v>13.92</v>
+      </c>
+      <c r="H28" t="n">
+        <v>19.6</v>
+      </c>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="b">
         <v>0</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>An error occurred. ... OSError(8, 'Exec format error')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C29" t="n">
-        <v>46387</v>
+        <v>10390</v>
       </c>
       <c r="D29" t="n">
-        <v>2469</v>
+        <v>554</v>
       </c>
       <c r="E29" t="n">
-        <v>5672</v>
+        <v>5174</v>
       </c>
       <c r="F29" t="n">
-        <v>357</v>
+        <v>408</v>
       </c>
       <c r="G29" t="n">
-        <v>12.23</v>
+        <v>49.8</v>
       </c>
       <c r="H29" t="n">
-        <v>14.46</v>
+        <v>73.65000000000001</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1572,32 +1532,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
         <v>44014</v>
       </c>
       <c r="C30" t="n">
-        <v>12504</v>
+        <v>33352</v>
       </c>
       <c r="D30" t="n">
+        <v>1701</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1794</v>
+      </c>
+      <c r="F30" t="n">
         <v>111</v>
       </c>
-      <c r="E30" t="n">
-        <v>464</v>
-      </c>
-      <c r="F30" t="n">
-        <v>17</v>
-      </c>
       <c r="G30" t="n">
-        <v>6.81</v>
+        <v>5.38</v>
       </c>
       <c r="H30" t="n">
-        <v>15.32</v>
+        <v>6.53</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="b">
         <v>0</v>
@@ -1611,16 +1571,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Montana</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C31" t="n">
+        <v>15207</v>
+      </c>
+      <c r="D31" t="n">
+        <v>377</v>
+      </c>
+      <c r="E31" t="n">
+        <v>542</v>
+      </c>
+      <c r="F31" t="n">
+        <v>12</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3.22</v>
+      </c>
       <c r="I31" t="b">
         <v>0</v>
       </c>
@@ -1629,39 +1603,39 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>An error occurred. ... SSLError(MaxRetryError("HTTPSConnectionPool(host='dphhs.mt.gov', port=443): Max retries exceeded with url: /publichealth/cdepi/diseases/coronavirusmt/demographics (Caused by SSLError(SSLError(1, '[SSL: DH_KEY_TOO_SMALL] dh key too small (_ssl.c:1108)')))"))</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="C32" t="n">
-        <v>29199</v>
+        <v>87709</v>
       </c>
       <c r="D32" t="n">
-        <v>786</v>
+        <v>2849</v>
       </c>
       <c r="E32" t="n">
-        <v>5085</v>
+        <v>24795</v>
       </c>
       <c r="F32" t="n">
-        <v>185</v>
+        <v>1350</v>
       </c>
       <c r="G32" t="n">
-        <v>19.43</v>
+        <v>28.27</v>
       </c>
       <c r="H32" t="n">
-        <v>23.87</v>
+        <v>47.39</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
@@ -1675,36 +1649,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
         <v>44014</v>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>212774</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>18519</t>
-        </is>
+      <c r="C33" t="n">
+        <v>63735</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1816</v>
       </c>
       <c r="E33" t="n">
-        <v>33093</v>
+        <v>9195</v>
       </c>
       <c r="F33" t="n">
-        <v>5171</v>
+        <v>396</v>
       </c>
       <c r="G33" t="n">
-        <v>30.17</v>
+        <v>14.43</v>
       </c>
       <c r="H33" t="n">
-        <v>30.48</v>
+        <v>21.81</v>
       </c>
       <c r="I33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
         <v>1</v>
@@ -1718,37 +1688,115 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C34" t="n">
+        <v>46387</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2469</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5672</v>
+      </c>
+      <c r="F34" t="n">
+        <v>357</v>
+      </c>
+      <c r="G34" t="n">
+        <v>12.23</v>
+      </c>
+      <c r="H34" t="n">
+        <v>14.46</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>44014</v>
+      </c>
+      <c r="C35" t="n">
+        <v>16079</v>
+      </c>
+      <c r="D35" t="n">
+        <v>581</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1590</v>
+      </c>
+      <c r="F35" t="n">
+        <v>86</v>
+      </c>
+      <c r="G35" t="n">
+        <v>14.55</v>
+      </c>
+      <c r="H35" t="n">
+        <v>15.84</v>
+      </c>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>California - Los Angeles</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n">
         <v>44013</v>
       </c>
-      <c r="C34" t="n">
-        <v>19310</v>
-      </c>
-      <c r="D34" t="n">
-        <v>276</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1122</v>
-      </c>
-      <c r="F34" t="n">
-        <v>21</v>
-      </c>
-      <c r="G34" t="n">
-        <v>7.59</v>
-      </c>
-      <c r="H34" t="n">
-        <v>7.95</v>
-      </c>
-      <c r="I34" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="inlineStr">
+      <c r="C36" t="n">
+        <v>107667</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3454</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2946</v>
+      </c>
+      <c r="F36" t="n">
+        <v>365</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="H36" t="n">
+        <v>10.57</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Success!</t>
         </is>

</xml_diff>